<commit_message>
changes done in the TestNG.xml file for 3rd time
</commit_message>
<xml_diff>
--- a/target/test-classes/data/PLSI_Automation_Data.xlsx
+++ b/target/test-classes/data/PLSI_Automation_Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SaiVamshi.Kotla.SSTECH\PLSIBaseFramework\PLSIAutomationBase\src\test\resources\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{817142F6-8EA1-4146-B7BF-9ACE9FC92CCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09B01625-BA9B-45C2-B347-4C2BBBBF785A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="5" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="4" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ReadMe" sheetId="1" r:id="rId1"/>
@@ -728,7 +728,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="17">
+  <fonts count="16">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -771,11 +771,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF6A8759"/>
-      <name val="Arial Unicode MS"/>
     </font>
     <font>
       <sz val="10"/>
@@ -918,7 +913,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -930,19 +925,16 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -960,8 +952,8 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="20" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -971,39 +963,39 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
@@ -1317,7 +1309,7 @@
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="39" t="s">
+      <c r="A2" s="38" t="s">
         <v>158</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -1326,7 +1318,7 @@
       <c r="C2" s="3"/>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" s="39" t="s">
+      <c r="A3" s="38" t="s">
         <v>161</v>
       </c>
       <c r="B3" s="2" t="s">
@@ -1335,7 +1327,7 @@
       <c r="C3" s="3"/>
     </row>
     <row r="4" spans="1:3">
-      <c r="A4" s="40" t="s">
+      <c r="A4" s="39" t="s">
         <v>63</v>
       </c>
       <c r="B4" s="2" t="s">
@@ -1343,7 +1335,7 @@
       </c>
     </row>
     <row r="5" spans="1:3">
-      <c r="A5" s="40" t="s">
+      <c r="A5" s="39" t="s">
         <v>64</v>
       </c>
       <c r="B5" s="2" t="s">
@@ -1351,7 +1343,7 @@
       </c>
     </row>
     <row r="6" spans="1:3">
-      <c r="A6" s="40" t="s">
+      <c r="A6" s="39" t="s">
         <v>65</v>
       </c>
       <c r="B6" s="2" t="s">
@@ -1359,7 +1351,7 @@
       </c>
     </row>
     <row r="7" spans="1:3">
-      <c r="A7" s="39" t="s">
+      <c r="A7" s="38" t="s">
         <v>162</v>
       </c>
       <c r="B7" s="2" t="s">
@@ -1367,7 +1359,7 @@
       </c>
     </row>
     <row r="8" spans="1:3">
-      <c r="A8" s="41" t="s">
+      <c r="A8" s="40" t="s">
         <v>184</v>
       </c>
       <c r="B8" s="2" t="s">
@@ -1375,7 +1367,7 @@
       </c>
     </row>
     <row r="9" spans="1:3">
-      <c r="A9" s="40" t="s">
+      <c r="A9" s="39" t="s">
         <v>92</v>
       </c>
       <c r="B9" s="2" t="s">
@@ -1383,7 +1375,7 @@
       </c>
     </row>
     <row r="10" spans="1:3">
-      <c r="A10" s="41" t="s">
+      <c r="A10" s="40" t="s">
         <v>185</v>
       </c>
       <c r="B10" s="2" t="s">
@@ -1391,7 +1383,7 @@
       </c>
     </row>
     <row r="11" spans="1:3">
-      <c r="A11" s="42" t="s">
+      <c r="A11" s="41" t="s">
         <v>128</v>
       </c>
       <c r="B11" s="2" t="s">
@@ -1399,7 +1391,7 @@
       </c>
     </row>
     <row r="12" spans="1:3">
-      <c r="A12" s="40" t="s">
+      <c r="A12" s="39" t="s">
         <v>78</v>
       </c>
       <c r="B12" s="2" t="s">
@@ -1407,7 +1399,7 @@
       </c>
     </row>
     <row r="13" spans="1:3">
-      <c r="A13" s="43" t="s">
+      <c r="A13" s="42" t="s">
         <v>81</v>
       </c>
       <c r="B13" s="2" t="s">
@@ -1415,7 +1407,7 @@
       </c>
     </row>
     <row r="14" spans="1:3">
-      <c r="A14" s="40" t="s">
+      <c r="A14" s="39" t="s">
         <v>82</v>
       </c>
       <c r="B14" s="2" t="s">
@@ -1423,7 +1415,7 @@
       </c>
     </row>
     <row r="15" spans="1:3">
-      <c r="A15" s="40" t="s">
+      <c r="A15" s="39" t="s">
         <v>84</v>
       </c>
       <c r="B15" s="2" t="s">
@@ -1431,7 +1423,7 @@
       </c>
     </row>
     <row r="16" spans="1:3">
-      <c r="A16" s="40" t="s">
+      <c r="A16" s="39" t="s">
         <v>85</v>
       </c>
       <c r="B16" s="2" t="s">
@@ -1439,7 +1431,7 @@
       </c>
     </row>
     <row r="17" spans="1:2">
-      <c r="A17" s="40" t="s">
+      <c r="A17" s="39" t="s">
         <v>86</v>
       </c>
       <c r="B17" s="2" t="s">
@@ -1447,7 +1439,7 @@
       </c>
     </row>
     <row r="18" spans="1:2">
-      <c r="A18" s="40" t="s">
+      <c r="A18" s="39" t="s">
         <v>195</v>
       </c>
       <c r="B18" s="2" t="s">
@@ -1455,7 +1447,7 @@
       </c>
     </row>
     <row r="19" spans="1:2">
-      <c r="A19" s="36" t="s">
+      <c r="A19" s="35" t="s">
         <v>200</v>
       </c>
       <c r="B19" s="2" t="s">
@@ -1463,7 +1455,7 @@
       </c>
     </row>
     <row r="20" spans="1:2">
-      <c r="A20" s="36" t="s">
+      <c r="A20" s="35" t="s">
         <v>199</v>
       </c>
       <c r="B20" s="2" t="s">
@@ -1471,7 +1463,7 @@
       </c>
     </row>
     <row r="21" spans="1:2">
-      <c r="A21" s="40" t="s">
+      <c r="A21" s="39" t="s">
         <v>74</v>
       </c>
       <c r="B21" s="2" t="s">
@@ -1479,7 +1471,7 @@
       </c>
     </row>
     <row r="22" spans="1:2">
-      <c r="A22" s="40" t="s">
+      <c r="A22" s="39" t="s">
         <v>75</v>
       </c>
       <c r="B22" s="2" t="s">
@@ -1487,7 +1479,7 @@
       </c>
     </row>
     <row r="23" spans="1:2">
-      <c r="A23" s="40" t="s">
+      <c r="A23" s="39" t="s">
         <v>76</v>
       </c>
       <c r="B23" s="2" t="s">
@@ -1495,7 +1487,7 @@
       </c>
     </row>
     <row r="24" spans="1:2">
-      <c r="A24" s="40" t="s">
+      <c r="A24" s="39" t="s">
         <v>73</v>
       </c>
       <c r="B24" s="2" t="s">
@@ -1503,7 +1495,7 @@
       </c>
     </row>
     <row r="25" spans="1:2">
-      <c r="A25" s="40" t="s">
+      <c r="A25" s="39" t="s">
         <v>95</v>
       </c>
       <c r="B25" s="2" t="s">
@@ -1511,7 +1503,7 @@
       </c>
     </row>
     <row r="26" spans="1:2">
-      <c r="A26" s="40" t="s">
+      <c r="A26" s="39" t="s">
         <v>98</v>
       </c>
       <c r="B26" s="2" t="s">
@@ -1519,7 +1511,7 @@
       </c>
     </row>
     <row r="27" spans="1:2">
-      <c r="A27" s="40" t="s">
+      <c r="A27" s="39" t="s">
         <v>101</v>
       </c>
       <c r="B27" s="2" t="s">
@@ -1527,7 +1519,7 @@
       </c>
     </row>
     <row r="28" spans="1:2">
-      <c r="A28" s="42" t="s">
+      <c r="A28" s="41" t="s">
         <v>192</v>
       </c>
       <c r="B28" s="2" t="s">
@@ -1535,7 +1527,7 @@
       </c>
     </row>
     <row r="29" spans="1:2">
-      <c r="A29" s="42" t="s">
+      <c r="A29" s="41" t="s">
         <v>173</v>
       </c>
       <c r="B29" s="2" t="s">
@@ -1543,7 +1535,7 @@
       </c>
     </row>
     <row r="30" spans="1:2">
-      <c r="A30" s="42" t="s">
+      <c r="A30" s="41" t="s">
         <v>165</v>
       </c>
       <c r="B30" s="2" t="s">
@@ -1551,7 +1543,7 @@
       </c>
     </row>
     <row r="31" spans="1:2">
-      <c r="A31" s="41" t="s">
+      <c r="A31" s="40" t="s">
         <v>191</v>
       </c>
       <c r="B31" s="2" t="s">
@@ -1559,7 +1551,7 @@
       </c>
     </row>
     <row r="32" spans="1:2">
-      <c r="A32" s="40" t="s">
+      <c r="A32" s="39" t="s">
         <v>166</v>
       </c>
       <c r="B32" s="2" t="s">
@@ -1567,7 +1559,7 @@
       </c>
     </row>
     <row r="33" spans="1:2">
-      <c r="A33" s="44" t="s">
+      <c r="A33" s="43" t="s">
         <v>104</v>
       </c>
       <c r="B33" s="2" t="s">
@@ -1575,7 +1567,7 @@
       </c>
     </row>
     <row r="34" spans="1:2">
-      <c r="A34" s="44" t="s">
+      <c r="A34" s="43" t="s">
         <v>107</v>
       </c>
       <c r="B34" s="2" t="s">
@@ -1583,7 +1575,7 @@
       </c>
     </row>
     <row r="35" spans="1:2">
-      <c r="A35" s="44" t="s">
+      <c r="A35" s="43" t="s">
         <v>108</v>
       </c>
       <c r="B35" s="2" t="s">
@@ -1591,7 +1583,7 @@
       </c>
     </row>
     <row r="36" spans="1:2">
-      <c r="A36" s="44" t="s">
+      <c r="A36" s="43" t="s">
         <v>110</v>
       </c>
       <c r="B36" s="2" t="s">
@@ -1599,7 +1591,7 @@
       </c>
     </row>
     <row r="37" spans="1:2" ht="28.8">
-      <c r="A37" s="44" t="s">
+      <c r="A37" s="43" t="s">
         <v>111</v>
       </c>
       <c r="B37" s="2" t="s">
@@ -1607,7 +1599,7 @@
       </c>
     </row>
     <row r="38" spans="1:2" ht="28.8">
-      <c r="A38" s="44" t="s">
+      <c r="A38" s="43" t="s">
         <v>112</v>
       </c>
       <c r="B38" s="2" t="s">
@@ -1615,7 +1607,7 @@
       </c>
     </row>
     <row r="39" spans="1:2">
-      <c r="A39" s="44" t="s">
+      <c r="A39" s="43" t="s">
         <v>113</v>
       </c>
       <c r="B39" s="2" t="s">
@@ -1623,7 +1615,7 @@
       </c>
     </row>
     <row r="40" spans="1:2">
-      <c r="A40" s="40" t="s">
+      <c r="A40" s="39" t="s">
         <v>190</v>
       </c>
       <c r="B40" s="2" t="s">
@@ -1631,7 +1623,7 @@
       </c>
     </row>
     <row r="41" spans="1:2">
-      <c r="A41" s="45" t="s">
+      <c r="A41" s="44" t="s">
         <v>186</v>
       </c>
       <c r="B41" s="2" t="s">
@@ -1639,7 +1631,7 @@
       </c>
     </row>
     <row r="42" spans="1:2">
-      <c r="A42" s="46" t="s">
+      <c r="A42" s="45" t="s">
         <v>193</v>
       </c>
       <c r="B42" s="2" t="s">
@@ -1647,7 +1639,7 @@
       </c>
     </row>
     <row r="43" spans="1:2">
-      <c r="A43" s="36" t="s">
+      <c r="A43" s="35" t="s">
         <v>202</v>
       </c>
       <c r="B43" s="2" t="s">
@@ -1665,7 +1657,7 @@
   <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1683,54 +1675,54 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="23" t="s">
         <v>60</v>
       </c>
-      <c r="B1" s="24" t="s">
+      <c r="B1" s="23" t="s">
         <v>62</v>
       </c>
-      <c r="C1" s="24" t="s">
+      <c r="C1" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="24" t="s">
+      <c r="D1" s="23" t="s">
         <v>167</v>
       </c>
-      <c r="E1" s="24" t="s">
+      <c r="E1" s="23" t="s">
         <v>168</v>
       </c>
-      <c r="F1" s="24" t="s">
+      <c r="F1" s="23" t="s">
         <v>169</v>
       </c>
-      <c r="G1" s="24" t="s">
+      <c r="G1" s="23" t="s">
         <v>118</v>
       </c>
-      <c r="H1" s="24" t="s">
+      <c r="H1" s="23" t="s">
         <v>163</v>
       </c>
-      <c r="I1" s="24" t="s">
+      <c r="I1" s="23" t="s">
         <v>164</v>
       </c>
-      <c r="J1" s="38" t="s">
+      <c r="J1" s="37" t="s">
         <v>188</v>
       </c>
     </row>
     <row r="2" spans="1:10">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="24" t="s">
         <v>192</v>
       </c>
-      <c r="B2" s="48" t="s">
+      <c r="B2" s="47" t="s">
         <v>226</v>
       </c>
-      <c r="C2" s="34" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="26" t="s">
+      <c r="C2" s="33" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="25" t="s">
         <v>170</v>
       </c>
-      <c r="E2" s="26" t="s">
+      <c r="E2" s="25" t="s">
         <v>171</v>
       </c>
-      <c r="F2" s="26" t="s">
+      <c r="F2" s="25" t="s">
         <v>172</v>
       </c>
       <c r="G2" t="s">
@@ -1747,13 +1739,13 @@
       </c>
     </row>
     <row r="3" spans="1:10">
-      <c r="A3" s="25" t="s">
+      <c r="A3" s="24" t="s">
         <v>173</v>
       </c>
-      <c r="B3" s="48" t="s">
+      <c r="B3" s="47" t="s">
         <v>226</v>
       </c>
-      <c r="C3" s="34" t="s">
+      <c r="C3" s="33" t="s">
         <v>2</v>
       </c>
       <c r="D3" t="s">
@@ -1779,13 +1771,13 @@
       </c>
     </row>
     <row r="4" spans="1:10">
-      <c r="A4" s="25" t="s">
+      <c r="A4" s="24" t="s">
         <v>165</v>
       </c>
-      <c r="B4" s="48" t="s">
+      <c r="B4" s="47" t="s">
         <v>227</v>
       </c>
-      <c r="C4" s="34" t="s">
+      <c r="C4" s="33" t="s">
         <v>2</v>
       </c>
       <c r="D4" t="s">
@@ -1797,13 +1789,13 @@
       <c r="F4" t="s">
         <v>129</v>
       </c>
-      <c r="G4" s="26" t="s">
+      <c r="G4" s="25" t="s">
         <v>39</v>
       </c>
-      <c r="H4" s="35" t="s">
+      <c r="H4" s="34" t="s">
         <v>175</v>
       </c>
-      <c r="I4" s="35" t="s">
+      <c r="I4" s="34" t="s">
         <v>174</v>
       </c>
       <c r="J4" t="s">
@@ -1814,10 +1806,10 @@
       <c r="A5" t="s">
         <v>166</v>
       </c>
-      <c r="B5" s="48" t="s">
+      <c r="B5" s="47" t="s">
         <v>227</v>
       </c>
-      <c r="C5" s="34" t="s">
+      <c r="C5" s="33" t="s">
         <v>2</v>
       </c>
       <c r="D5" t="s">
@@ -1843,7 +1835,7 @@
       </c>
     </row>
     <row r="6" spans="1:10">
-      <c r="A6" s="36" t="s">
+      <c r="A6" s="35" t="s">
         <v>191</v>
       </c>
       <c r="B6" s="4" t="s">
@@ -1956,7 +1948,7 @@
       </c>
     </row>
     <row r="2" spans="1:13">
-      <c r="A2" s="36" t="s">
+      <c r="A2" s="35" t="s">
         <v>202</v>
       </c>
       <c r="B2" t="s">
@@ -1980,10 +1972,10 @@
       <c r="H2" t="s">
         <v>221</v>
       </c>
-      <c r="I2" s="21" t="s">
+      <c r="I2" s="20" t="s">
         <v>216</v>
       </c>
-      <c r="J2" s="21" t="s">
+      <c r="J2" s="20" t="s">
         <v>217</v>
       </c>
       <c r="K2" t="s">
@@ -1992,7 +1984,7 @@
       <c r="L2" t="s">
         <v>219</v>
       </c>
-      <c r="M2" s="21" t="s">
+      <c r="M2" s="20" t="s">
         <v>215</v>
       </c>
     </row>
@@ -2007,7 +1999,7 @@
   <dimension ref="A1:S7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -2033,7 +2025,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" s="6" customFormat="1">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="23" t="s">
         <v>60</v>
       </c>
       <c r="B1" s="8" t="s">
@@ -2069,22 +2061,22 @@
       <c r="L1" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="M1" s="22" t="s">
+      <c r="M1" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="N1" s="22" t="s">
+      <c r="N1" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="O1" s="22" t="s">
+      <c r="O1" s="21" t="s">
         <v>67</v>
       </c>
-      <c r="P1" s="22" t="s">
+      <c r="P1" s="21" t="s">
         <v>27</v>
       </c>
       <c r="Q1" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="R1" s="23" t="s">
+      <c r="R1" s="22" t="s">
         <v>119</v>
       </c>
       <c r="S1" s="6" t="s">
@@ -2092,50 +2084,50 @@
       </c>
     </row>
     <row r="2" spans="1:19">
-      <c r="A2" s="37" t="s">
+      <c r="A2" s="36" t="s">
         <v>184</v>
       </c>
-      <c r="B2" s="49" t="s">
+      <c r="B2" s="48" t="s">
         <v>226</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>2</v>
       </c>
       <c r="D2" s="4"/>
-      <c r="E2" s="26" t="s">
+      <c r="E2" s="25" t="s">
         <v>121</v>
       </c>
-      <c r="F2" s="26" t="s">
+      <c r="F2" s="25" t="s">
         <v>68</v>
       </c>
-      <c r="G2" s="26" t="s">
+      <c r="G2" s="25" t="s">
         <v>69</v>
       </c>
-      <c r="H2" s="25" t="s">
+      <c r="H2" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="I2" s="25" t="s">
+      <c r="I2" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="J2" s="25" t="s">
+      <c r="J2" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="K2" s="25" t="s">
+      <c r="K2" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="L2" s="25" t="s">
+      <c r="L2" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="M2" s="25" t="s">
+      <c r="M2" s="24" t="s">
         <v>70</v>
       </c>
-      <c r="N2" s="25" t="s">
+      <c r="N2" s="24" t="s">
         <v>89</v>
       </c>
-      <c r="O2" s="25" t="s">
+      <c r="O2" s="24" t="s">
         <v>90</v>
       </c>
-      <c r="P2" s="26" t="s">
+      <c r="P2" s="25" t="s">
         <v>71</v>
       </c>
       <c r="Q2" t="s">
@@ -2149,7 +2141,7 @@
       <c r="A3" t="s">
         <v>92</v>
       </c>
-      <c r="B3" s="49" t="s">
+      <c r="B3" s="48" t="s">
         <v>226</v>
       </c>
       <c r="C3" s="4" t="s">
@@ -2163,7 +2155,7 @@
       <c r="A4" t="s">
         <v>185</v>
       </c>
-      <c r="B4" s="49" t="s">
+      <c r="B4" s="48" t="s">
         <v>226</v>
       </c>
       <c r="C4" s="4" t="s">
@@ -2172,40 +2164,40 @@
       <c r="D4" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="E4" s="26" t="s">
+      <c r="E4" s="25" t="s">
         <v>91</v>
       </c>
-      <c r="F4" s="26" t="s">
+      <c r="F4" s="25" t="s">
         <v>68</v>
       </c>
-      <c r="G4" s="26" t="s">
+      <c r="G4" s="25" t="s">
         <v>69</v>
       </c>
-      <c r="H4" s="25" t="s">
+      <c r="H4" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="I4" s="25" t="s">
+      <c r="I4" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="J4" s="25" t="s">
+      <c r="J4" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="K4" s="25" t="s">
+      <c r="K4" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="L4" s="25" t="s">
+      <c r="L4" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="M4" s="25" t="s">
+      <c r="M4" s="24" t="s">
         <v>124</v>
       </c>
-      <c r="N4" s="25" t="s">
+      <c r="N4" s="24" t="s">
         <v>125</v>
       </c>
-      <c r="O4" s="25" t="s">
+      <c r="O4" s="24" t="s">
         <v>126</v>
       </c>
-      <c r="P4" s="26" t="s">
+      <c r="P4" s="25" t="s">
         <v>71</v>
       </c>
       <c r="Q4" t="s">
@@ -2216,10 +2208,10 @@
       </c>
     </row>
     <row r="5" spans="1:19">
-      <c r="A5" s="25" t="s">
+      <c r="A5" s="24" t="s">
         <v>128</v>
       </c>
-      <c r="B5" s="49" t="s">
+      <c r="B5" s="48" t="s">
         <v>226</v>
       </c>
       <c r="C5" s="4" t="s">
@@ -2231,10 +2223,10 @@
       <c r="E5" t="s">
         <v>129</v>
       </c>
-      <c r="F5" s="26" t="s">
+      <c r="F5" s="25" t="s">
         <v>130</v>
       </c>
-      <c r="G5" s="26" t="s">
+      <c r="G5" s="25" t="s">
         <v>131</v>
       </c>
       <c r="H5" t="s">
@@ -2278,7 +2270,7 @@
       <c r="A6" t="s">
         <v>190</v>
       </c>
-      <c r="B6" s="49" t="s">
+      <c r="B6" s="48" t="s">
         <v>226</v>
       </c>
       <c r="C6" t="s">
@@ -2328,10 +2320,10 @@
       </c>
     </row>
     <row r="7" spans="1:19">
-      <c r="A7" s="17" t="s">
+      <c r="A7" s="16" t="s">
         <v>193</v>
       </c>
-      <c r="B7" s="49" t="s">
+      <c r="B7" s="48" t="s">
         <v>226</v>
       </c>
       <c r="C7" s="4" t="s">
@@ -2340,40 +2332,40 @@
       <c r="D7" t="s">
         <v>129</v>
       </c>
-      <c r="E7" s="26" t="s">
-        <v>129</v>
-      </c>
-      <c r="F7" s="26" t="s">
+      <c r="E7" s="25" t="s">
+        <v>129</v>
+      </c>
+      <c r="F7" s="25" t="s">
         <v>68</v>
       </c>
-      <c r="G7" s="26" t="s">
+      <c r="G7" s="25" t="s">
         <v>69</v>
       </c>
-      <c r="H7" s="25" t="s">
+      <c r="H7" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="I7" s="25" t="s">
+      <c r="I7" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="J7" s="25" t="s">
+      <c r="J7" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="K7" s="25" t="s">
+      <c r="K7" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="L7" s="25" t="s">
+      <c r="L7" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="M7" s="25" t="s">
+      <c r="M7" s="24" t="s">
         <v>194</v>
       </c>
-      <c r="N7" s="25" t="s">
+      <c r="N7" s="24" t="s">
         <v>224</v>
       </c>
-      <c r="O7" s="25" t="s">
+      <c r="O7" s="24" t="s">
         <v>90</v>
       </c>
-      <c r="P7" s="26" t="s">
+      <c r="P7" s="25" t="s">
         <v>71</v>
       </c>
       <c r="Q7" t="s">
@@ -2403,7 +2395,7 @@
   <dimension ref="A1:AD8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -2449,233 +2441,233 @@
       <c r="G1" s="8" t="s">
         <v>136</v>
       </c>
-      <c r="H1" s="27" t="s">
+      <c r="H1" s="26" t="s">
         <v>137</v>
       </c>
-      <c r="I1" s="27" t="s">
+      <c r="I1" s="26" t="s">
         <v>138</v>
       </c>
-      <c r="J1" s="27" t="s">
+      <c r="J1" s="26" t="s">
         <v>139</v>
       </c>
-      <c r="K1" s="27" t="s">
+      <c r="K1" s="26" t="s">
         <v>140</v>
       </c>
-      <c r="L1" s="27" t="s">
+      <c r="L1" s="26" t="s">
         <v>141</v>
       </c>
-      <c r="M1" s="27" t="s">
+      <c r="M1" s="26" t="s">
         <v>142</v>
       </c>
-      <c r="N1" s="27" t="s">
+      <c r="N1" s="26" t="s">
         <v>143</v>
       </c>
-      <c r="O1" s="27" t="s">
+      <c r="O1" s="26" t="s">
         <v>144</v>
       </c>
-      <c r="P1" s="27" t="s">
+      <c r="P1" s="26" t="s">
         <v>145</v>
       </c>
-      <c r="Q1" s="27" t="s">
+      <c r="Q1" s="26" t="s">
         <v>146</v>
       </c>
-      <c r="R1" s="27" t="s">
+      <c r="R1" s="26" t="s">
         <v>147</v>
       </c>
-      <c r="S1" s="27" t="s">
+      <c r="S1" s="26" t="s">
         <v>148</v>
       </c>
-      <c r="T1" s="27" t="s">
+      <c r="T1" s="26" t="s">
         <v>149</v>
       </c>
-      <c r="U1" s="27" t="s">
+      <c r="U1" s="26" t="s">
         <v>150</v>
       </c>
-      <c r="V1" s="27" t="s">
+      <c r="V1" s="26" t="s">
         <v>151</v>
       </c>
-      <c r="W1" s="27" t="s">
+      <c r="W1" s="26" t="s">
         <v>152</v>
       </c>
-      <c r="X1" s="27" t="s">
+      <c r="X1" s="26" t="s">
         <v>153</v>
       </c>
-      <c r="Y1" s="27" t="s">
+      <c r="Y1" s="26" t="s">
         <v>154</v>
       </c>
-      <c r="Z1" s="27" t="s">
+      <c r="Z1" s="26" t="s">
         <v>155</v>
       </c>
-      <c r="AA1" s="27" t="s">
+      <c r="AA1" s="26" t="s">
         <v>156</v>
       </c>
-      <c r="AB1" s="27" t="s">
+      <c r="AB1" s="26" t="s">
         <v>157</v>
       </c>
     </row>
     <row r="2" spans="1:30">
-      <c r="A2" s="28" t="s">
+      <c r="A2" s="27" t="s">
         <v>158</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="47" t="s">
+        <v>226</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="28">
+        <v>0.73749999999999993</v>
+      </c>
+      <c r="E2" s="28">
+        <v>0.78472222222222221</v>
+      </c>
+      <c r="F2" s="29">
+        <v>2.65</v>
+      </c>
+      <c r="G2" s="30" t="s">
+        <v>159</v>
+      </c>
+      <c r="H2" s="31">
         <v>1</v>
       </c>
-      <c r="C2" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="29">
+      <c r="I2" s="31">
+        <v>1</v>
+      </c>
+      <c r="J2" s="31">
+        <v>170</v>
+      </c>
+      <c r="K2" s="31">
+        <v>2</v>
+      </c>
+      <c r="L2" s="31">
+        <v>2</v>
+      </c>
+      <c r="M2" s="31">
+        <v>1</v>
+      </c>
+      <c r="N2" s="31">
+        <v>60</v>
+      </c>
+      <c r="O2" s="31">
+        <v>5</v>
+      </c>
+      <c r="P2" s="31">
+        <v>4</v>
+      </c>
+      <c r="Q2" s="31">
+        <v>3</v>
+      </c>
+      <c r="R2" s="31">
+        <v>20</v>
+      </c>
+      <c r="S2" s="32" t="s">
+        <v>160</v>
+      </c>
+      <c r="T2" s="31">
+        <v>1.25</v>
+      </c>
+      <c r="U2" s="31">
+        <v>1.5</v>
+      </c>
+      <c r="V2" s="32"/>
+      <c r="W2" s="32"/>
+      <c r="X2" s="31">
+        <v>7</v>
+      </c>
+      <c r="Y2" s="31">
+        <v>3</v>
+      </c>
+      <c r="Z2" s="31">
+        <v>40</v>
+      </c>
+      <c r="AA2" s="31">
+        <v>5</v>
+      </c>
+      <c r="AB2" s="31">
+        <v>120</v>
+      </c>
+      <c r="AC2" s="30"/>
+      <c r="AD2" s="30"/>
+    </row>
+    <row r="3" spans="1:30">
+      <c r="A3" s="27" t="s">
+        <v>161</v>
+      </c>
+      <c r="B3" s="47" t="s">
+        <v>226</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="28">
         <v>0.73749999999999993</v>
       </c>
-      <c r="E2" s="29">
+      <c r="E3" s="28">
         <v>0.78472222222222221</v>
       </c>
-      <c r="F2" s="30">
+      <c r="F3" s="29">
         <v>2.65</v>
       </c>
-      <c r="G2" s="31" t="s">
+      <c r="G3" s="30" t="s">
         <v>159</v>
       </c>
-      <c r="H2" s="32">
+      <c r="H3" s="31">
         <v>1</v>
       </c>
-      <c r="I2" s="32">
+      <c r="I3" s="31">
         <v>1</v>
       </c>
-      <c r="J2" s="32">
+      <c r="J3" s="31">
         <v>170</v>
       </c>
-      <c r="K2" s="32">
-        <v>2</v>
-      </c>
-      <c r="L2" s="32">
-        <v>2</v>
-      </c>
-      <c r="M2" s="32">
+      <c r="K3" s="31">
+        <v>2</v>
+      </c>
+      <c r="L3" s="31">
+        <v>2</v>
+      </c>
+      <c r="M3" s="31">
         <v>1</v>
       </c>
-      <c r="N2" s="32">
+      <c r="N3" s="31">
         <v>60</v>
       </c>
-      <c r="O2" s="32">
+      <c r="O3" s="31">
         <v>5</v>
       </c>
-      <c r="P2" s="32">
+      <c r="P3" s="31">
         <v>4</v>
       </c>
-      <c r="Q2" s="32">
+      <c r="Q3" s="31">
         <v>3</v>
       </c>
-      <c r="R2" s="32">
+      <c r="R3" s="31">
         <v>20</v>
       </c>
-      <c r="S2" s="33" t="s">
+      <c r="S3" s="32" t="s">
         <v>160</v>
       </c>
-      <c r="T2" s="32">
+      <c r="T3" s="31">
         <v>1.25</v>
       </c>
-      <c r="U2" s="32">
+      <c r="U3" s="31">
         <v>1.5</v>
       </c>
-      <c r="V2" s="33"/>
-      <c r="W2" s="33"/>
-      <c r="X2" s="32">
+      <c r="V3" s="32"/>
+      <c r="W3" s="32"/>
+      <c r="X3" s="31">
         <v>7</v>
       </c>
-      <c r="Y2" s="32">
+      <c r="Y3" s="31">
         <v>3</v>
       </c>
-      <c r="Z2" s="32">
+      <c r="Z3" s="31">
         <v>40</v>
       </c>
-      <c r="AA2" s="32">
+      <c r="AA3" s="31">
         <v>5</v>
       </c>
-      <c r="AB2" s="32">
-        <v>120</v>
-      </c>
-      <c r="AC2" s="31"/>
-      <c r="AD2" s="31"/>
-    </row>
-    <row r="3" spans="1:30">
-      <c r="A3" s="28" t="s">
-        <v>161</v>
-      </c>
-      <c r="B3" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" s="29">
-        <v>0.73749999999999993</v>
-      </c>
-      <c r="E3" s="29">
-        <v>0.78472222222222221</v>
-      </c>
-      <c r="F3" s="30">
-        <v>2.65</v>
-      </c>
-      <c r="G3" s="31" t="s">
-        <v>159</v>
-      </c>
-      <c r="H3" s="32">
-        <v>1</v>
-      </c>
-      <c r="I3" s="32">
-        <v>1</v>
-      </c>
-      <c r="J3" s="32">
-        <v>170</v>
-      </c>
-      <c r="K3" s="32">
-        <v>2</v>
-      </c>
-      <c r="L3" s="32">
-        <v>2</v>
-      </c>
-      <c r="M3" s="32">
-        <v>1</v>
-      </c>
-      <c r="N3" s="32">
-        <v>60</v>
-      </c>
-      <c r="O3" s="32">
-        <v>5</v>
-      </c>
-      <c r="P3" s="32">
-        <v>4</v>
-      </c>
-      <c r="Q3" s="32">
-        <v>3</v>
-      </c>
-      <c r="R3" s="32">
-        <v>20</v>
-      </c>
-      <c r="S3" s="33" t="s">
-        <v>160</v>
-      </c>
-      <c r="T3" s="32">
-        <v>1.25</v>
-      </c>
-      <c r="U3" s="32">
-        <v>1.5</v>
-      </c>
-      <c r="V3" s="33"/>
-      <c r="W3" s="33"/>
-      <c r="X3" s="32">
-        <v>7</v>
-      </c>
-      <c r="Y3" s="32">
-        <v>3</v>
-      </c>
-      <c r="Z3" s="32">
-        <v>40</v>
-      </c>
-      <c r="AA3" s="32">
-        <v>5</v>
-      </c>
-      <c r="AB3" s="32">
+      <c r="AB3" s="31">
         <v>120</v>
       </c>
       <c r="AC3" s="7"/>
@@ -2685,8 +2677,8 @@
       <c r="A4" t="s">
         <v>63</v>
       </c>
-      <c r="B4" s="11" t="s">
-        <v>1</v>
+      <c r="B4" s="47" t="s">
+        <v>225</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>2</v>
@@ -2696,8 +2688,8 @@
       <c r="A5" t="s">
         <v>64</v>
       </c>
-      <c r="B5" s="11" t="s">
-        <v>1</v>
+      <c r="B5" s="47" t="s">
+        <v>225</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>2</v>
@@ -2707,19 +2699,19 @@
       <c r="A6" t="s">
         <v>65</v>
       </c>
-      <c r="B6" s="11" t="s">
-        <v>1</v>
+      <c r="B6" s="47" t="s">
+        <v>225</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:30">
-      <c r="A7" s="28" t="s">
+      <c r="A7" s="27" t="s">
         <v>162</v>
       </c>
-      <c r="B7" s="11" t="s">
-        <v>1</v>
+      <c r="B7" s="47" t="s">
+        <v>225</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>2</v>
@@ -2729,11 +2721,11 @@
       </c>
     </row>
     <row r="8" spans="1:30">
-      <c r="A8" s="28" t="s">
+      <c r="A8" s="27" t="s">
         <v>186</v>
       </c>
-      <c r="B8" s="11" t="s">
-        <v>1</v>
+      <c r="B8" s="47" t="s">
+        <v>225</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>2</v>
@@ -2748,9 +2740,13 @@
     <hyperlink ref="C3" r:id="rId5" xr:uid="{3FD6D116-216A-4423-835A-F97000FF95CC}"/>
     <hyperlink ref="C7" r:id="rId6" xr:uid="{E7BB4DFE-A00A-494B-B573-2FA848FA84CF}"/>
     <hyperlink ref="C8" r:id="rId7" xr:uid="{AADD8828-4D21-4908-9221-0DCFA4071DA4}"/>
+    <hyperlink ref="B2" r:id="rId8" xr:uid="{702090F1-D65E-4B43-8116-49D16CD7A344}"/>
+    <hyperlink ref="B4" r:id="rId9" xr:uid="{19B58D5C-E0A0-4C0E-8D70-E2D8E7A9F58E}"/>
+    <hyperlink ref="B5:B7" r:id="rId10" display="gangadhar.m@sstech.us" xr:uid="{656BAC6F-28F9-4DC5-8F87-75919D119C60}"/>
+    <hyperlink ref="B8" r:id="rId11" xr:uid="{7083E1D2-F435-446C-ACA8-690E33C58B84}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId8"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId12"/>
 </worksheet>
 </file>
 
@@ -2776,35 +2772,35 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="C1" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="D1" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="E1" s="13" t="s">
+      <c r="E1" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="F1" s="13" t="s">
+      <c r="F1" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="G1" s="13" t="s">
+      <c r="G1" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="H1" s="13" t="s">
+      <c r="H1" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="I1" s="13" t="s">
+      <c r="I1" s="12" t="s">
         <v>176</v>
       </c>
-      <c r="J1" s="13"/>
-      <c r="K1" s="13"/>
+      <c r="J1" s="12"/>
+      <c r="K1" s="12"/>
     </row>
     <row r="2" spans="1:11">
       <c r="A2" t="s">
@@ -2816,7 +2812,7 @@
       <c r="C2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="15" t="s">
+      <c r="D2" s="14" t="s">
         <v>109</v>
       </c>
       <c r="E2" s="4" t="s">
@@ -2833,7 +2829,7 @@
       </c>
     </row>
     <row r="3" spans="1:11">
-      <c r="A3" s="14" t="s">
+      <c r="A3" s="13" t="s">
         <v>81</v>
       </c>
       <c r="B3" s="4" t="s">
@@ -2842,7 +2838,7 @@
       <c r="C3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="15" t="s">
+      <c r="D3" s="14" t="s">
         <v>109</v>
       </c>
       <c r="E3" s="4" t="s">
@@ -2868,7 +2864,7 @@
       <c r="C4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="15" t="s">
+      <c r="D4" s="14" t="s">
         <v>109</v>
       </c>
       <c r="E4" s="4" t="s">
@@ -2894,7 +2890,7 @@
       <c r="C5" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="15" t="s">
+      <c r="D5" s="14" t="s">
         <v>109</v>
       </c>
       <c r="E5" s="4" t="s">
@@ -2920,7 +2916,7 @@
       <c r="C6" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="15" t="s">
+      <c r="D6" s="14" t="s">
         <v>109</v>
       </c>
       <c r="E6" s="4" t="s">
@@ -2949,7 +2945,7 @@
       <c r="C7" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D7" s="15" t="s">
+      <c r="D7" s="14" t="s">
         <v>109</v>
       </c>
       <c r="E7" s="4" t="s">
@@ -2992,7 +2988,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="16" type="noConversion"/>
+  <phoneticPr fontId="15" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="E2" r:id="rId1" xr:uid="{0D458867-A002-45E1-B365-545961492A16}"/>
     <hyperlink ref="E3:E7" r:id="rId2" display="deepa.pattar@sstech.us" xr:uid="{61492ADE-3336-44E6-9318-42D2D7523F4D}"/>
@@ -3100,7 +3096,7 @@
       </c>
     </row>
     <row r="2" spans="1:20">
-      <c r="A2" s="36" t="s">
+      <c r="A2" s="35" t="s">
         <v>200</v>
       </c>
       <c r="B2" s="4" t="s">
@@ -3142,7 +3138,7 @@
       <c r="N2" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="O2" s="47" t="s">
+      <c r="O2" s="46" t="s">
         <v>197</v>
       </c>
       <c r="P2" t="s">
@@ -3162,7 +3158,7 @@
       </c>
     </row>
     <row r="3" spans="1:20">
-      <c r="A3" s="36" t="s">
+      <c r="A3" s="35" t="s">
         <v>199</v>
       </c>
       <c r="B3" s="4" t="s">
@@ -3204,7 +3200,7 @@
       <c r="N3" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="O3" s="47" t="s">
+      <c r="O3" s="46" t="s">
         <v>198</v>
       </c>
       <c r="P3" t="s">
@@ -3242,7 +3238,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BB21362-C935-4D70-8A2D-2CFAFF7C4674}">
   <dimension ref="A1:M2"/>
   <sheetViews>
-    <sheetView topLeftCell="W1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="Q15" sqref="Q15"/>
     </sheetView>
   </sheetViews>
@@ -3355,7 +3351,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC50B798-C00F-4686-80C0-D4DC574A8857}">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
@@ -3368,16 +3364,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="11" t="s">
         <v>188</v>
       </c>
     </row>
@@ -3391,7 +3387,7 @@
       <c r="C2" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="15" t="s">
+      <c r="D2" s="14" t="s">
         <v>109</v>
       </c>
     </row>
@@ -3405,7 +3401,7 @@
       <c r="C3" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="15" t="s">
+      <c r="D3" s="14" t="s">
         <v>109</v>
       </c>
     </row>
@@ -3419,7 +3415,7 @@
       <c r="C4" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="15" t="s">
+      <c r="D4" s="14" t="s">
         <v>109</v>
       </c>
     </row>
@@ -3453,8 +3449,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C956B14F-0A4B-4BD7-A86C-D911C2214633}">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -3476,61 +3472,61 @@
       <c r="C1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="16" t="s">
+      <c r="D1" s="15" t="s">
         <v>93</v>
       </c>
-      <c r="E1" s="16" t="s">
+      <c r="E1" s="15" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="16" t="s">
         <v>95</v>
       </c>
-      <c r="B2" s="11" t="s">
-        <v>1</v>
+      <c r="B2" s="48" t="s">
+        <v>226</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="18" t="s">
+      <c r="D2" s="17" t="s">
         <v>96</v>
       </c>
-      <c r="E2" s="18" t="s">
+      <c r="E2" s="17" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" s="17" t="s">
+      <c r="A3" s="16" t="s">
         <v>98</v>
       </c>
-      <c r="B3" s="11" t="s">
-        <v>1</v>
+      <c r="B3" s="48" t="s">
+        <v>226</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="18" t="s">
+      <c r="D3" s="17" t="s">
         <v>99</v>
       </c>
-      <c r="E3" s="18" t="s">
+      <c r="E3" s="17" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" s="17" t="s">
+      <c r="A4" s="16" t="s">
         <v>101</v>
       </c>
-      <c r="B4" s="11" t="s">
-        <v>1</v>
+      <c r="B4" s="48" t="s">
+        <v>226</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="18" t="s">
+      <c r="D4" s="17" t="s">
         <v>102</v>
       </c>
-      <c r="E4" s="18" t="s">
+      <c r="E4" s="17" t="s">
         <v>103</v>
       </c>
     </row>
@@ -3539,6 +3535,8 @@
     <hyperlink ref="C2" r:id="rId1" xr:uid="{D9097781-0FAD-493C-9670-CEA54F22237C}"/>
     <hyperlink ref="C3" r:id="rId2" xr:uid="{048F86AF-02A7-43B2-9117-5783D566A05C}"/>
     <hyperlink ref="C4" r:id="rId3" xr:uid="{42365D77-69E6-4644-A553-C7BF1E28C142}"/>
+    <hyperlink ref="B2" r:id="rId4" xr:uid="{9255B575-F868-46AC-A994-F6C2E6BD1D30}"/>
+    <hyperlink ref="B3:B4" r:id="rId5" display="sravani.bandaru@sstech.us" xr:uid="{9A70ECE9-620A-480D-BEB1-C52794BEB28E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3549,7 +3547,7 @@
   <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -3564,37 +3562,37 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="19" t="s">
         <v>60</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="C1" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="D1" s="12" t="s">
         <v>114</v>
       </c>
-      <c r="E1" s="13" t="s">
+      <c r="E1" s="12" t="s">
         <v>115</v>
       </c>
-      <c r="F1" s="13" t="s">
+      <c r="F1" s="12" t="s">
         <v>116</v>
       </c>
-      <c r="G1" s="13" t="s">
+      <c r="G1" s="12" t="s">
         <v>117</v>
       </c>
-      <c r="H1" s="13" t="s">
+      <c r="H1" s="12" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="18" t="s">
         <v>104</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>1</v>
+      <c r="B2" s="47" t="s">
+        <v>226</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>2</v>
@@ -3605,16 +3603,16 @@
       <c r="E2" t="s">
         <v>105</v>
       </c>
-      <c r="F2" s="21" t="s">
+      <c r="F2" s="20" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="3" spans="1:8">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="18" t="s">
         <v>107</v>
       </c>
-      <c r="B3" t="s">
-        <v>1</v>
+      <c r="B3" s="47" t="s">
+        <v>226</v>
       </c>
       <c r="C3" t="s">
         <v>2</v>
@@ -3627,11 +3625,11 @@
       </c>
     </row>
     <row r="4" spans="1:8">
-      <c r="A4" s="19" t="s">
+      <c r="A4" s="18" t="s">
         <v>108</v>
       </c>
-      <c r="B4" t="s">
-        <v>1</v>
+      <c r="B4" s="47" t="s">
+        <v>226</v>
       </c>
       <c r="C4" t="s">
         <v>2</v>
@@ -3644,11 +3642,11 @@
       </c>
     </row>
     <row r="5" spans="1:8">
-      <c r="A5" s="19" t="s">
+      <c r="A5" s="18" t="s">
         <v>110</v>
       </c>
-      <c r="B5" t="s">
-        <v>1</v>
+      <c r="B5" s="47" t="s">
+        <v>226</v>
       </c>
       <c r="C5" t="s">
         <v>2</v>
@@ -3661,16 +3659,16 @@
       </c>
     </row>
     <row r="6" spans="1:8" ht="28.8">
-      <c r="A6" s="19" t="s">
+      <c r="A6" s="18" t="s">
         <v>111</v>
       </c>
-      <c r="B6" t="s">
-        <v>1</v>
+      <c r="B6" s="47" t="s">
+        <v>226</v>
       </c>
       <c r="C6" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="19" t="s">
+      <c r="D6" s="18" t="s">
         <v>109</v>
       </c>
       <c r="E6" t="s">
@@ -3678,11 +3676,11 @@
       </c>
     </row>
     <row r="7" spans="1:8" ht="28.8">
-      <c r="A7" s="19" t="s">
+      <c r="A7" s="18" t="s">
         <v>112</v>
       </c>
-      <c r="B7" t="s">
-        <v>1</v>
+      <c r="B7" s="47" t="s">
+        <v>226</v>
       </c>
       <c r="C7" t="s">
         <v>2</v>
@@ -3695,11 +3693,11 @@
       </c>
     </row>
     <row r="8" spans="1:8">
-      <c r="A8" s="19" t="s">
+      <c r="A8" s="18" t="s">
         <v>113</v>
       </c>
-      <c r="B8" t="s">
-        <v>1</v>
+      <c r="B8" s="47" t="s">
+        <v>226</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>2</v>
@@ -3718,14 +3716,15 @@
       </c>
     </row>
     <row r="9" spans="1:8">
-      <c r="A9" s="19"/>
+      <c r="A9" s="18"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C12" r:id="rId1" display="Welcome@1" xr:uid="{8F3E35E5-FF30-420A-BFB6-FDD10921CC00}"/>
-    <hyperlink ref="B2" r:id="rId2" xr:uid="{B3C73D34-948D-4F1D-8BAC-27F416656071}"/>
-    <hyperlink ref="C2" r:id="rId3" xr:uid="{A32E531E-3F0E-4487-9740-6966412A252F}"/>
-    <hyperlink ref="C8" r:id="rId4" xr:uid="{8F3E35E5-FF30-420A-BFB6-FDD10921CC00}"/>
+    <hyperlink ref="C2" r:id="rId2" xr:uid="{A32E531E-3F0E-4487-9740-6966412A252F}"/>
+    <hyperlink ref="C8" r:id="rId3" xr:uid="{8F3E35E5-FF30-420A-BFB6-FDD10921CC00}"/>
+    <hyperlink ref="B2" r:id="rId4" xr:uid="{D0354CD3-973B-4571-A569-36FB285BD704}"/>
+    <hyperlink ref="B3:B8" r:id="rId5" display="sravani.bandaru@sstech.us" xr:uid="{FA92DD12-C0DD-4D29-BB7C-89104C0625E1}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>